<commit_message>
update package datasets, add gg_ex_bar object
</commit_message>
<xml_diff>
--- a/data-raw/summary_data_for_ggplot.xlsx
+++ b/data-raw/summary_data_for_ggplot.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\egrid_ggplot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ggcapdthemes\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30D1D2A2-C5CA-46FC-B812-88A16E849E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57E3D39-85C8-450C-8ABC-AFF758BFD6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="260" windowWidth="19200" windowHeight="9940" xr2:uid="{F1CFC80A-1627-4E7B-B737-0980B0395894}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F1CFC80A-1627-4E7B-B737-0980B0395894}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -85,9 +74,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="#,##0.0%"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +118,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -156,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -237,13 +232,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -256,13 +281,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -600,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D541180-34C2-486E-87E2-E2C84971F253}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,154 +691,154 @@
     </row>
     <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2022</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1281209</v>
-      </c>
-      <c r="C2" s="1">
-        <v>4240140533</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="E2" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="G2" s="2">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1303568.8</v>
+      </c>
+      <c r="C2" s="12">
+        <v>4167601391.1820002</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E2" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="G2" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.182</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="H2" s="13">
+        <v>0.186</v>
+      </c>
+      <c r="I2" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="J2" s="2">
-        <v>1.2E-2</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="L2" s="2">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="M2" s="2">
+      <c r="J2" s="13">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="L2" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="M2" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="14">
         <v>1E-3</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2021</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1258286</v>
-      </c>
-      <c r="C3" s="7">
-        <v>4120144619.3579998</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.219</v>
-      </c>
-      <c r="E3" s="8">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.38400000000000001</v>
-      </c>
-      <c r="G3" s="8">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1281209</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4240140533</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="G3" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H3" s="8">
-        <v>0.189</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.06</v>
-      </c>
-      <c r="J3" s="8">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="K3" s="8">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L3" s="8">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="M3" s="8">
+      <c r="H3" s="2">
+        <v>0.182</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="M3" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="3">
         <v>1E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2020</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1656188</v>
-      </c>
-      <c r="C4" s="1">
-        <v>4021549453</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.193</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="G4" s="2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="I4" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="K4" s="2">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="L4" s="2">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="M4" s="2">
+        <v>2021</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1258286</v>
+      </c>
+      <c r="C4" s="7">
+        <v>4120144619.3579998</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.219</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.189</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="K4" s="8">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="L4" s="8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="M4" s="8">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="9">
         <v>1E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B5" s="1">
-        <v>1613477</v>
+        <v>1656188</v>
       </c>
       <c r="C5" s="1">
-        <v>4140185857</v>
+        <v>4021549453</v>
       </c>
       <c r="D5" s="2">
-        <v>0.23300000000000001</v>
+        <v>0.193</v>
       </c>
       <c r="E5" s="2">
-        <v>6.0000000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>0.38400000000000001</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="G5" s="2">
         <v>3.0000000000000001E-3</v>
@@ -813,16 +847,16 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="I5" s="2">
-        <v>6.8000000000000005E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J5" s="2">
-        <v>1.6E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K5" s="2">
-        <v>7.0999999999999994E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="L5" s="2">
-        <v>1.7000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M5" s="2">
         <v>4.0000000000000001E-3</v>
@@ -831,47 +865,91 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B6" s="1">
-        <v>1561643</v>
+        <v>1613477</v>
       </c>
       <c r="C6" s="1">
-        <v>4168370118</v>
+        <v>4140185857</v>
       </c>
       <c r="D6" s="2">
-        <v>0.27500000000000002</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="E6" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F6" s="2">
-        <v>0.35099999999999998</v>
+        <v>0.38400000000000001</v>
       </c>
       <c r="G6" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="H6" s="2">
-        <v>0.19400000000000001</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I6" s="2">
-        <v>6.9000000000000006E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="J6" s="2">
         <v>1.6E-2</v>
       </c>
       <c r="K6" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="L6" s="2">
-        <v>1.4999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="M6" s="2">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="N6" s="3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2018</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1561643</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4168370118</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M7" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N7" s="3">
         <v>1E-3</v>
       </c>
     </row>

</xml_diff>